<commit_message>
desde work 08 Ago
</commit_message>
<xml_diff>
--- a/Consultores/04. PLANILLAS SUELDOS REGENTES 2025.xlsx
+++ b/Consultores/04. PLANILLAS SUELDOS REGENTES 2025.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="102">
   <si>
     <t xml:space="preserve">GOBIERNO AUTONOMO MUNICIPAL DE SACABA</t>
   </si>
@@ -623,183 +623,183 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -807,83 +807,83 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="3" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -898,47 +898,6 @@
     <cellStyle name="Normal 2" xfId="20"/>
     <cellStyle name="Normal 4" xfId="21"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0CECE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1013,9 +972,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2733120</xdr:colOff>
+      <xdr:colOff>2732760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1028,8 +987,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21699720" y="0"/>
-          <a:ext cx="830160" cy="752040"/>
+          <a:off x="21700440" y="0"/>
+          <a:ext cx="829800" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1055,9 +1014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2733120</xdr:colOff>
+      <xdr:colOff>2732760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1070,8 +1029,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21071160" y="0"/>
-          <a:ext cx="830160" cy="752040"/>
+          <a:off x="21071880" y="0"/>
+          <a:ext cx="829800" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1097,9 +1056,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2733120</xdr:colOff>
+      <xdr:colOff>2732760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1112,8 +1071,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21494160" y="0"/>
-          <a:ext cx="830160" cy="752040"/>
+          <a:off x="21495240" y="0"/>
+          <a:ext cx="829800" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1139,9 +1098,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2733120</xdr:colOff>
+      <xdr:colOff>2732760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1154,8 +1113,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21699720" y="0"/>
-          <a:ext cx="830160" cy="752040"/>
+          <a:off x="21700440" y="0"/>
+          <a:ext cx="829800" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1181,9 +1140,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2733120</xdr:colOff>
+      <xdr:colOff>2732760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1196,8 +1155,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21699720" y="0"/>
-          <a:ext cx="830160" cy="752040"/>
+          <a:off x="21700440" y="0"/>
+          <a:ext cx="829800" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1223,9 +1182,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2733120</xdr:colOff>
+      <xdr:colOff>2732760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1238,8 +1197,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21699720" y="0"/>
-          <a:ext cx="830160" cy="752040"/>
+          <a:off x="21700440" y="0"/>
+          <a:ext cx="829800" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1265,9 +1224,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2733120</xdr:colOff>
+      <xdr:colOff>2732760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1280,8 +1239,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21699720" y="0"/>
-          <a:ext cx="830160" cy="752040"/>
+          <a:off x="21700440" y="0"/>
+          <a:ext cx="829800" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1478,7 +1437,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="H16" activeCellId="1" sqref="33:36 H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1490,8 +1449,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="3" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="14.29"/>
@@ -7054,7 +7013,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="1" sqref="33:36 A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7066,8 +7025,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="3" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="14.29"/>
@@ -12596,20 +12555,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="H14" activeCellId="1" sqref="33:36 H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="5.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="3" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="14.29"/>
@@ -15890,7 +15849,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="P15" activeCellId="1" sqref="33:36 P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15902,8 +15861,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="3" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="14.29"/>
@@ -22047,7 +22006,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="10" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="1" sqref="33:36 A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22059,8 +22018,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="3" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="14.29"/>
@@ -28036,12 +27995,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:DV32"/>
+  <dimension ref="A1:XFD36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="10" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="10" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="33:36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28053,8 +28012,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="3" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="14.29"/>
@@ -33988,8 +33947,1733 @@
       <c r="DU32" s="66"/>
       <c r="DV32" s="66"/>
     </row>
+    <row r="33" s="50" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="51"/>
+      <c r="W33" s="51"/>
+      <c r="X33" s="51"/>
+      <c r="Y33" s="51"/>
+      <c r="Z33" s="51"/>
+      <c r="AA33" s="51"/>
+      <c r="AB33" s="51"/>
+      <c r="AC33" s="51"/>
+      <c r="AD33" s="51"/>
+      <c r="AE33" s="51"/>
+      <c r="AF33" s="51"/>
+      <c r="AG33" s="51"/>
+      <c r="AH33" s="51"/>
+      <c r="AI33" s="51"/>
+      <c r="AJ33" s="51"/>
+      <c r="AK33" s="51"/>
+      <c r="AL33" s="51"/>
+      <c r="AM33" s="51"/>
+      <c r="AN33" s="51"/>
+      <c r="AO33" s="51"/>
+      <c r="AP33" s="51"/>
+      <c r="AQ33" s="51"/>
+      <c r="AR33" s="51"/>
+      <c r="AS33" s="51"/>
+      <c r="AT33" s="51"/>
+      <c r="AU33" s="51"/>
+      <c r="AV33" s="51"/>
+      <c r="AW33" s="51"/>
+      <c r="AX33" s="51"/>
+      <c r="AY33" s="51"/>
+      <c r="AZ33" s="51"/>
+      <c r="BA33" s="51"/>
+      <c r="BB33" s="51"/>
+      <c r="BC33" s="51"/>
+      <c r="BD33" s="51"/>
+      <c r="BE33" s="51"/>
+      <c r="BF33" s="51"/>
+      <c r="BG33" s="51"/>
+      <c r="BH33" s="51"/>
+      <c r="BI33" s="51"/>
+      <c r="BJ33" s="51"/>
+      <c r="BK33" s="51"/>
+      <c r="BL33" s="51"/>
+      <c r="BM33" s="51"/>
+      <c r="BN33" s="51"/>
+      <c r="BO33" s="51"/>
+      <c r="BP33" s="51"/>
+      <c r="BQ33" s="51"/>
+      <c r="BR33" s="51"/>
+      <c r="BS33" s="51"/>
+      <c r="BT33" s="51"/>
+      <c r="BU33" s="51"/>
+      <c r="BV33" s="51"/>
+      <c r="BW33" s="51"/>
+      <c r="BX33" s="51"/>
+      <c r="BY33" s="51"/>
+      <c r="BZ33" s="51"/>
+      <c r="CA33" s="51"/>
+      <c r="CB33" s="51"/>
+      <c r="CC33" s="51"/>
+      <c r="CD33" s="51"/>
+      <c r="CE33" s="51"/>
+      <c r="CF33" s="51"/>
+      <c r="CG33" s="51"/>
+      <c r="CH33" s="51"/>
+      <c r="CI33" s="51"/>
+      <c r="CJ33" s="51"/>
+      <c r="CK33" s="51"/>
+      <c r="CL33" s="51"/>
+      <c r="CM33" s="51"/>
+      <c r="CN33" s="51"/>
+      <c r="CO33" s="51"/>
+      <c r="CP33" s="51"/>
+      <c r="CQ33" s="51"/>
+      <c r="CR33" s="51"/>
+      <c r="CS33" s="51"/>
+      <c r="CT33" s="51"/>
+      <c r="CU33" s="51"/>
+      <c r="CV33" s="51"/>
+      <c r="CW33" s="51"/>
+      <c r="CX33" s="51"/>
+      <c r="CY33" s="51"/>
+      <c r="CZ33" s="51"/>
+      <c r="DA33" s="51"/>
+      <c r="DB33" s="51"/>
+      <c r="DC33" s="51"/>
+      <c r="DD33" s="51"/>
+      <c r="DE33" s="51"/>
+      <c r="DF33" s="51"/>
+      <c r="DG33" s="51"/>
+      <c r="DH33" s="51"/>
+      <c r="DI33" s="51"/>
+      <c r="DJ33" s="51"/>
+      <c r="DK33" s="51"/>
+      <c r="DL33" s="51"/>
+      <c r="DM33" s="51"/>
+      <c r="DN33" s="51"/>
+      <c r="DO33" s="51"/>
+      <c r="DP33" s="51"/>
+      <c r="DQ33" s="51"/>
+      <c r="DR33" s="51"/>
+      <c r="DS33" s="51"/>
+      <c r="DT33" s="51"/>
+      <c r="DU33" s="51"/>
+      <c r="DV33" s="51"/>
+      <c r="WUK33" s="0"/>
+      <c r="WUL33" s="0"/>
+      <c r="WUM33" s="0"/>
+      <c r="WUN33" s="0"/>
+      <c r="WUO33" s="0"/>
+      <c r="WUP33" s="0"/>
+      <c r="WUQ33" s="0"/>
+      <c r="WUR33" s="0"/>
+      <c r="WUS33" s="0"/>
+      <c r="WUT33" s="0"/>
+      <c r="WUU33" s="0"/>
+      <c r="WUV33" s="0"/>
+      <c r="WUW33" s="0"/>
+      <c r="WUX33" s="0"/>
+      <c r="WUY33" s="0"/>
+      <c r="WUZ33" s="0"/>
+      <c r="WVA33" s="0"/>
+      <c r="WVB33" s="0"/>
+      <c r="WVC33" s="0"/>
+      <c r="WVD33" s="0"/>
+      <c r="WVE33" s="0"/>
+      <c r="WVF33" s="0"/>
+      <c r="WVG33" s="0"/>
+      <c r="WVH33" s="0"/>
+      <c r="WVI33" s="0"/>
+      <c r="WVJ33" s="0"/>
+      <c r="WVK33" s="0"/>
+      <c r="WVL33" s="0"/>
+      <c r="WVM33" s="0"/>
+      <c r="WVN33" s="0"/>
+      <c r="WVO33" s="0"/>
+      <c r="WVP33" s="0"/>
+      <c r="WVQ33" s="0"/>
+      <c r="WVR33" s="0"/>
+      <c r="WVS33" s="0"/>
+      <c r="WVT33" s="0"/>
+      <c r="WVU33" s="0"/>
+      <c r="WVV33" s="0"/>
+      <c r="WVW33" s="0"/>
+      <c r="WVX33" s="0"/>
+      <c r="WVY33" s="0"/>
+      <c r="WVZ33" s="0"/>
+      <c r="WWA33" s="0"/>
+      <c r="WWB33" s="0"/>
+      <c r="WWC33" s="0"/>
+      <c r="WWD33" s="0"/>
+      <c r="WWE33" s="0"/>
+      <c r="WWF33" s="0"/>
+      <c r="WWG33" s="0"/>
+      <c r="WWH33" s="0"/>
+      <c r="WWI33" s="0"/>
+      <c r="WWJ33" s="0"/>
+      <c r="WWK33" s="0"/>
+      <c r="WWL33" s="0"/>
+      <c r="WWM33" s="0"/>
+      <c r="WWN33" s="0"/>
+      <c r="WWO33" s="0"/>
+      <c r="WWP33" s="0"/>
+      <c r="WWQ33" s="0"/>
+      <c r="WWR33" s="0"/>
+      <c r="WWS33" s="0"/>
+      <c r="WWT33" s="0"/>
+      <c r="WWU33" s="0"/>
+      <c r="WWV33" s="0"/>
+      <c r="WWW33" s="0"/>
+      <c r="WWX33" s="0"/>
+      <c r="WWY33" s="0"/>
+      <c r="WWZ33" s="0"/>
+      <c r="WXA33" s="0"/>
+      <c r="WXB33" s="0"/>
+      <c r="WXC33" s="0"/>
+      <c r="WXD33" s="0"/>
+      <c r="WXE33" s="0"/>
+      <c r="WXF33" s="0"/>
+      <c r="WXG33" s="0"/>
+      <c r="WXH33" s="0"/>
+      <c r="WXI33" s="0"/>
+      <c r="WXJ33" s="0"/>
+      <c r="WXK33" s="0"/>
+      <c r="WXL33" s="0"/>
+      <c r="WXM33" s="0"/>
+      <c r="WXN33" s="0"/>
+      <c r="WXO33" s="0"/>
+      <c r="WXP33" s="0"/>
+      <c r="WXQ33" s="0"/>
+      <c r="WXR33" s="0"/>
+      <c r="WXS33" s="0"/>
+      <c r="WXT33" s="0"/>
+      <c r="WXU33" s="0"/>
+      <c r="WXV33" s="0"/>
+      <c r="WXW33" s="0"/>
+      <c r="WXX33" s="0"/>
+      <c r="WXY33" s="0"/>
+      <c r="WXZ33" s="0"/>
+      <c r="WYA33" s="0"/>
+      <c r="WYB33" s="0"/>
+      <c r="WYC33" s="0"/>
+      <c r="WYD33" s="0"/>
+      <c r="WYE33" s="0"/>
+      <c r="WYF33" s="0"/>
+      <c r="WYG33" s="0"/>
+      <c r="WYH33" s="0"/>
+      <c r="WYI33" s="0"/>
+      <c r="WYJ33" s="0"/>
+      <c r="WYK33" s="0"/>
+      <c r="WYL33" s="0"/>
+      <c r="WYM33" s="0"/>
+      <c r="WYN33" s="0"/>
+      <c r="WYO33" s="0"/>
+      <c r="WYP33" s="0"/>
+      <c r="WYQ33" s="0"/>
+      <c r="WYR33" s="0"/>
+      <c r="WYS33" s="0"/>
+      <c r="WYT33" s="0"/>
+      <c r="WYU33" s="0"/>
+      <c r="WYV33" s="0"/>
+      <c r="WYW33" s="0"/>
+      <c r="WYX33" s="0"/>
+      <c r="WYY33" s="0"/>
+      <c r="WYZ33" s="0"/>
+      <c r="WZA33" s="0"/>
+      <c r="WZB33" s="0"/>
+      <c r="WZC33" s="0"/>
+      <c r="WZD33" s="0"/>
+      <c r="WZE33" s="0"/>
+      <c r="WZF33" s="0"/>
+      <c r="WZG33" s="0"/>
+      <c r="WZH33" s="0"/>
+      <c r="WZI33" s="0"/>
+      <c r="WZJ33" s="0"/>
+      <c r="WZK33" s="0"/>
+      <c r="WZL33" s="0"/>
+      <c r="WZM33" s="0"/>
+      <c r="WZN33" s="0"/>
+      <c r="WZO33" s="0"/>
+      <c r="WZP33" s="0"/>
+      <c r="WZQ33" s="0"/>
+      <c r="WZR33" s="0"/>
+      <c r="WZS33" s="0"/>
+      <c r="WZT33" s="0"/>
+      <c r="WZU33" s="0"/>
+      <c r="WZV33" s="0"/>
+      <c r="WZW33" s="0"/>
+      <c r="WZX33" s="0"/>
+      <c r="WZY33" s="0"/>
+      <c r="WZZ33" s="0"/>
+      <c r="XAA33" s="0"/>
+      <c r="XAB33" s="0"/>
+      <c r="XAC33" s="0"/>
+      <c r="XAD33" s="0"/>
+      <c r="XAE33" s="0"/>
+      <c r="XAF33" s="0"/>
+      <c r="XAG33" s="0"/>
+      <c r="XAH33" s="0"/>
+      <c r="XAI33" s="0"/>
+      <c r="XAJ33" s="0"/>
+      <c r="XAK33" s="0"/>
+      <c r="XAL33" s="0"/>
+      <c r="XAM33" s="0"/>
+      <c r="XAN33" s="0"/>
+      <c r="XAO33" s="0"/>
+      <c r="XAP33" s="0"/>
+      <c r="XAQ33" s="0"/>
+      <c r="XAR33" s="0"/>
+      <c r="XAS33" s="0"/>
+      <c r="XAT33" s="0"/>
+      <c r="XAU33" s="0"/>
+      <c r="XAV33" s="0"/>
+      <c r="XAW33" s="0"/>
+      <c r="XAX33" s="0"/>
+      <c r="XAY33" s="0"/>
+      <c r="XAZ33" s="0"/>
+      <c r="XBA33" s="0"/>
+      <c r="XBB33" s="0"/>
+      <c r="XBC33" s="0"/>
+      <c r="XBD33" s="0"/>
+      <c r="XBE33" s="0"/>
+      <c r="XBF33" s="0"/>
+      <c r="XBG33" s="0"/>
+      <c r="XBH33" s="0"/>
+      <c r="XBI33" s="0"/>
+      <c r="XBJ33" s="0"/>
+      <c r="XBK33" s="0"/>
+      <c r="XBL33" s="0"/>
+      <c r="XBM33" s="0"/>
+      <c r="XBN33" s="0"/>
+      <c r="XBO33" s="0"/>
+      <c r="XBP33" s="0"/>
+      <c r="XBQ33" s="0"/>
+      <c r="XBR33" s="0"/>
+      <c r="XBS33" s="0"/>
+      <c r="XBT33" s="0"/>
+      <c r="XBU33" s="0"/>
+      <c r="XBV33" s="0"/>
+      <c r="XBW33" s="0"/>
+      <c r="XBX33" s="0"/>
+      <c r="XBY33" s="0"/>
+      <c r="XBZ33" s="0"/>
+      <c r="XCA33" s="0"/>
+      <c r="XCB33" s="0"/>
+      <c r="XCC33" s="0"/>
+      <c r="XCD33" s="0"/>
+      <c r="XCE33" s="0"/>
+      <c r="XCF33" s="0"/>
+      <c r="XCG33" s="0"/>
+      <c r="XCH33" s="0"/>
+      <c r="XCI33" s="0"/>
+      <c r="XCJ33" s="0"/>
+      <c r="XCK33" s="0"/>
+      <c r="XCL33" s="0"/>
+      <c r="XCM33" s="0"/>
+      <c r="XCN33" s="0"/>
+      <c r="XCO33" s="0"/>
+      <c r="XCP33" s="0"/>
+      <c r="XCQ33" s="0"/>
+      <c r="XCR33" s="0"/>
+      <c r="XCS33" s="0"/>
+      <c r="XCT33" s="0"/>
+      <c r="XCU33" s="0"/>
+      <c r="XCV33" s="0"/>
+      <c r="XCW33" s="0"/>
+      <c r="XCX33" s="0"/>
+      <c r="XCY33" s="0"/>
+      <c r="XCZ33" s="0"/>
+      <c r="XDA33" s="0"/>
+      <c r="XDB33" s="0"/>
+      <c r="XDC33" s="0"/>
+      <c r="XDD33" s="0"/>
+      <c r="XDE33" s="0"/>
+      <c r="XDF33" s="0"/>
+      <c r="XDG33" s="0"/>
+      <c r="XDH33" s="0"/>
+      <c r="XDI33" s="0"/>
+      <c r="XDJ33" s="0"/>
+      <c r="XDK33" s="0"/>
+      <c r="XDL33" s="0"/>
+      <c r="XDM33" s="0"/>
+      <c r="XDN33" s="0"/>
+      <c r="XDO33" s="0"/>
+      <c r="XDP33" s="0"/>
+      <c r="XDQ33" s="0"/>
+      <c r="XDR33" s="0"/>
+      <c r="XDS33" s="0"/>
+      <c r="XDT33" s="0"/>
+      <c r="XDU33" s="0"/>
+      <c r="XDV33" s="0"/>
+      <c r="XDW33" s="0"/>
+      <c r="XDX33" s="0"/>
+      <c r="XDY33" s="0"/>
+      <c r="XDZ33" s="0"/>
+      <c r="XEA33" s="0"/>
+      <c r="XEB33" s="0"/>
+      <c r="XEC33" s="0"/>
+      <c r="XED33" s="0"/>
+      <c r="XEE33" s="0"/>
+      <c r="XEF33" s="0"/>
+      <c r="XEG33" s="0"/>
+      <c r="XEH33" s="0"/>
+      <c r="XEI33" s="0"/>
+      <c r="XEJ33" s="0"/>
+      <c r="XEK33" s="0"/>
+      <c r="XEL33" s="0"/>
+      <c r="XEM33" s="0"/>
+      <c r="XEN33" s="0"/>
+      <c r="XEO33" s="0"/>
+      <c r="XEP33" s="0"/>
+      <c r="XEQ33" s="0"/>
+      <c r="XER33" s="0"/>
+      <c r="XES33" s="0"/>
+      <c r="XET33" s="0"/>
+      <c r="XEU33" s="0"/>
+      <c r="XEV33" s="0"/>
+      <c r="XEW33" s="0"/>
+      <c r="XEX33" s="0"/>
+      <c r="XEY33" s="0"/>
+      <c r="XEZ33" s="0"/>
+      <c r="XFA33" s="0"/>
+      <c r="XFB33" s="0"/>
+      <c r="XFC33" s="0"/>
+      <c r="XFD33" s="0"/>
+    </row>
+    <row r="34" s="61" customFormat="true" ht="75.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="53" t="n">
+        <v>14094029</v>
+      </c>
+      <c r="E34" s="54" t="n">
+        <v>35960</v>
+      </c>
+      <c r="F34" s="52"/>
+      <c r="G34" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" s="54" t="n">
+        <v>45824</v>
+      </c>
+      <c r="J34" s="54" t="n">
+        <v>45993</v>
+      </c>
+      <c r="K34" s="57" t="n">
+        <v>15</v>
+      </c>
+      <c r="L34" s="58" t="n">
+        <v>2000</v>
+      </c>
+      <c r="M34" s="59" t="n">
+        <f aca="false">ROUND(L34/30*K34,2)</f>
+        <v>1000</v>
+      </c>
+      <c r="N34" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" s="59" t="n">
+        <f aca="false">ROUND(M34-Q34,2)</f>
+        <v>1000</v>
+      </c>
+      <c r="S34" s="52"/>
+      <c r="U34" s="62"/>
+      <c r="V34" s="62"/>
+      <c r="W34" s="62"/>
+      <c r="X34" s="62"/>
+      <c r="Y34" s="62"/>
+      <c r="Z34" s="62"/>
+      <c r="AA34" s="62"/>
+      <c r="AB34" s="62"/>
+      <c r="AC34" s="62"/>
+      <c r="AD34" s="62"/>
+      <c r="AE34" s="62"/>
+      <c r="AF34" s="62"/>
+      <c r="AG34" s="62"/>
+      <c r="AH34" s="62"/>
+      <c r="AI34" s="62"/>
+      <c r="AJ34" s="62"/>
+      <c r="AK34" s="62"/>
+      <c r="AL34" s="62"/>
+      <c r="AM34" s="62"/>
+      <c r="AN34" s="62"/>
+      <c r="AO34" s="62"/>
+      <c r="AP34" s="62"/>
+      <c r="AQ34" s="62"/>
+      <c r="AR34" s="62"/>
+      <c r="AS34" s="62"/>
+      <c r="AT34" s="62"/>
+      <c r="AU34" s="62"/>
+      <c r="AV34" s="62"/>
+      <c r="AW34" s="62"/>
+      <c r="AX34" s="62"/>
+      <c r="AY34" s="62"/>
+      <c r="AZ34" s="62"/>
+      <c r="BA34" s="62"/>
+      <c r="BB34" s="62"/>
+      <c r="BC34" s="62"/>
+      <c r="BD34" s="62"/>
+      <c r="BE34" s="62"/>
+      <c r="BF34" s="62"/>
+      <c r="BG34" s="62"/>
+      <c r="BH34" s="62"/>
+      <c r="BI34" s="62"/>
+      <c r="BJ34" s="62"/>
+      <c r="BK34" s="62"/>
+      <c r="BL34" s="62"/>
+      <c r="BM34" s="62"/>
+      <c r="BN34" s="62"/>
+      <c r="BO34" s="62"/>
+      <c r="BP34" s="62"/>
+      <c r="BQ34" s="62"/>
+      <c r="BR34" s="62"/>
+      <c r="BS34" s="62"/>
+      <c r="BT34" s="62"/>
+      <c r="BU34" s="62"/>
+      <c r="BV34" s="62"/>
+      <c r="BW34" s="62"/>
+      <c r="BX34" s="62"/>
+      <c r="BY34" s="62"/>
+      <c r="BZ34" s="62"/>
+      <c r="CA34" s="62"/>
+      <c r="CB34" s="62"/>
+      <c r="CC34" s="62"/>
+      <c r="CD34" s="62"/>
+      <c r="CE34" s="62"/>
+      <c r="CF34" s="62"/>
+      <c r="CG34" s="62"/>
+      <c r="CH34" s="62"/>
+      <c r="CI34" s="62"/>
+      <c r="CJ34" s="62"/>
+      <c r="CK34" s="62"/>
+      <c r="CL34" s="62"/>
+      <c r="CM34" s="62"/>
+      <c r="CN34" s="62"/>
+      <c r="CO34" s="62"/>
+      <c r="CP34" s="62"/>
+      <c r="CQ34" s="62"/>
+      <c r="CR34" s="62"/>
+      <c r="CS34" s="62"/>
+      <c r="CT34" s="62"/>
+      <c r="CU34" s="62"/>
+      <c r="CV34" s="62"/>
+      <c r="CW34" s="62"/>
+      <c r="CX34" s="62"/>
+      <c r="CY34" s="62"/>
+      <c r="CZ34" s="62"/>
+      <c r="DA34" s="62"/>
+      <c r="DB34" s="62"/>
+      <c r="DC34" s="62"/>
+      <c r="DD34" s="62"/>
+      <c r="DE34" s="62"/>
+      <c r="DF34" s="62"/>
+      <c r="DG34" s="62"/>
+      <c r="DH34" s="62"/>
+      <c r="DI34" s="62"/>
+      <c r="DJ34" s="62"/>
+      <c r="DK34" s="62"/>
+      <c r="DL34" s="62"/>
+      <c r="DM34" s="62"/>
+      <c r="DN34" s="62"/>
+      <c r="DO34" s="62"/>
+      <c r="DP34" s="62"/>
+      <c r="DQ34" s="62"/>
+      <c r="DR34" s="62"/>
+      <c r="DS34" s="62"/>
+      <c r="DT34" s="62"/>
+      <c r="DU34" s="62"/>
+      <c r="DV34" s="62"/>
+      <c r="WUK34" s="0"/>
+      <c r="WUL34" s="0"/>
+      <c r="WUM34" s="0"/>
+      <c r="WUN34" s="0"/>
+      <c r="WUO34" s="0"/>
+      <c r="WUP34" s="0"/>
+      <c r="WUQ34" s="0"/>
+      <c r="WUR34" s="0"/>
+      <c r="WUS34" s="0"/>
+      <c r="WUT34" s="0"/>
+      <c r="WUU34" s="0"/>
+      <c r="WUV34" s="0"/>
+      <c r="WUW34" s="0"/>
+      <c r="WUX34" s="0"/>
+      <c r="WUY34" s="0"/>
+      <c r="WUZ34" s="0"/>
+      <c r="WVA34" s="0"/>
+      <c r="WVB34" s="0"/>
+      <c r="WVC34" s="0"/>
+      <c r="WVD34" s="0"/>
+      <c r="WVE34" s="0"/>
+      <c r="WVF34" s="0"/>
+      <c r="WVG34" s="0"/>
+      <c r="WVH34" s="0"/>
+      <c r="WVI34" s="0"/>
+      <c r="WVJ34" s="0"/>
+      <c r="WVK34" s="0"/>
+      <c r="WVL34" s="0"/>
+      <c r="WVM34" s="0"/>
+      <c r="WVN34" s="0"/>
+      <c r="WVO34" s="0"/>
+      <c r="WVP34" s="0"/>
+      <c r="WVQ34" s="0"/>
+      <c r="WVR34" s="0"/>
+      <c r="WVS34" s="0"/>
+      <c r="WVT34" s="0"/>
+      <c r="WVU34" s="0"/>
+      <c r="WVV34" s="0"/>
+      <c r="WVW34" s="0"/>
+      <c r="WVX34" s="0"/>
+      <c r="WVY34" s="0"/>
+      <c r="WVZ34" s="0"/>
+      <c r="WWA34" s="0"/>
+      <c r="WWB34" s="0"/>
+      <c r="WWC34" s="0"/>
+      <c r="WWD34" s="0"/>
+      <c r="WWE34" s="0"/>
+      <c r="WWF34" s="0"/>
+      <c r="WWG34" s="0"/>
+      <c r="WWH34" s="0"/>
+      <c r="WWI34" s="0"/>
+      <c r="WWJ34" s="0"/>
+      <c r="WWK34" s="0"/>
+      <c r="WWL34" s="0"/>
+      <c r="WWM34" s="0"/>
+      <c r="WWN34" s="0"/>
+      <c r="WWO34" s="0"/>
+      <c r="WWP34" s="0"/>
+      <c r="WWQ34" s="0"/>
+      <c r="WWR34" s="0"/>
+      <c r="WWS34" s="0"/>
+      <c r="WWT34" s="0"/>
+      <c r="WWU34" s="0"/>
+      <c r="WWV34" s="0"/>
+      <c r="WWW34" s="0"/>
+      <c r="WWX34" s="0"/>
+      <c r="WWY34" s="0"/>
+      <c r="WWZ34" s="0"/>
+      <c r="WXA34" s="0"/>
+      <c r="WXB34" s="0"/>
+      <c r="WXC34" s="0"/>
+      <c r="WXD34" s="0"/>
+      <c r="WXE34" s="0"/>
+      <c r="WXF34" s="0"/>
+      <c r="WXG34" s="0"/>
+      <c r="WXH34" s="0"/>
+      <c r="WXI34" s="0"/>
+      <c r="WXJ34" s="0"/>
+      <c r="WXK34" s="0"/>
+      <c r="WXL34" s="0"/>
+      <c r="WXM34" s="0"/>
+      <c r="WXN34" s="0"/>
+      <c r="WXO34" s="0"/>
+      <c r="WXP34" s="0"/>
+      <c r="WXQ34" s="0"/>
+      <c r="WXR34" s="0"/>
+      <c r="WXS34" s="0"/>
+      <c r="WXT34" s="0"/>
+      <c r="WXU34" s="0"/>
+      <c r="WXV34" s="0"/>
+      <c r="WXW34" s="0"/>
+      <c r="WXX34" s="0"/>
+      <c r="WXY34" s="0"/>
+      <c r="WXZ34" s="0"/>
+      <c r="WYA34" s="0"/>
+      <c r="WYB34" s="0"/>
+      <c r="WYC34" s="0"/>
+      <c r="WYD34" s="0"/>
+      <c r="WYE34" s="0"/>
+      <c r="WYF34" s="0"/>
+      <c r="WYG34" s="0"/>
+      <c r="WYH34" s="0"/>
+      <c r="WYI34" s="0"/>
+      <c r="WYJ34" s="0"/>
+      <c r="WYK34" s="0"/>
+      <c r="WYL34" s="0"/>
+      <c r="WYM34" s="0"/>
+      <c r="WYN34" s="0"/>
+      <c r="WYO34" s="0"/>
+      <c r="WYP34" s="0"/>
+      <c r="WYQ34" s="0"/>
+      <c r="WYR34" s="0"/>
+      <c r="WYS34" s="0"/>
+      <c r="WYT34" s="0"/>
+      <c r="WYU34" s="0"/>
+      <c r="WYV34" s="0"/>
+      <c r="WYW34" s="0"/>
+      <c r="WYX34" s="0"/>
+      <c r="WYY34" s="0"/>
+      <c r="WYZ34" s="0"/>
+      <c r="WZA34" s="0"/>
+      <c r="WZB34" s="0"/>
+      <c r="WZC34" s="0"/>
+      <c r="WZD34" s="0"/>
+      <c r="WZE34" s="0"/>
+      <c r="WZF34" s="0"/>
+      <c r="WZG34" s="0"/>
+      <c r="WZH34" s="0"/>
+      <c r="WZI34" s="0"/>
+      <c r="WZJ34" s="0"/>
+      <c r="WZK34" s="0"/>
+      <c r="WZL34" s="0"/>
+      <c r="WZM34" s="0"/>
+      <c r="WZN34" s="0"/>
+      <c r="WZO34" s="0"/>
+      <c r="WZP34" s="0"/>
+      <c r="WZQ34" s="0"/>
+      <c r="WZR34" s="0"/>
+      <c r="WZS34" s="0"/>
+      <c r="WZT34" s="0"/>
+      <c r="WZU34" s="0"/>
+      <c r="WZV34" s="0"/>
+      <c r="WZW34" s="0"/>
+      <c r="WZX34" s="0"/>
+      <c r="WZY34" s="0"/>
+      <c r="WZZ34" s="0"/>
+      <c r="XAA34" s="0"/>
+      <c r="XAB34" s="0"/>
+      <c r="XAC34" s="0"/>
+      <c r="XAD34" s="0"/>
+      <c r="XAE34" s="0"/>
+      <c r="XAF34" s="0"/>
+      <c r="XAG34" s="0"/>
+      <c r="XAH34" s="0"/>
+      <c r="XAI34" s="0"/>
+      <c r="XAJ34" s="0"/>
+      <c r="XAK34" s="0"/>
+      <c r="XAL34" s="0"/>
+      <c r="XAM34" s="0"/>
+      <c r="XAN34" s="0"/>
+      <c r="XAO34" s="0"/>
+      <c r="XAP34" s="0"/>
+      <c r="XAQ34" s="0"/>
+      <c r="XAR34" s="0"/>
+      <c r="XAS34" s="0"/>
+      <c r="XAT34" s="0"/>
+      <c r="XAU34" s="0"/>
+      <c r="XAV34" s="0"/>
+      <c r="XAW34" s="0"/>
+      <c r="XAX34" s="0"/>
+      <c r="XAY34" s="0"/>
+      <c r="XAZ34" s="0"/>
+      <c r="XBA34" s="0"/>
+      <c r="XBB34" s="0"/>
+      <c r="XBC34" s="0"/>
+      <c r="XBD34" s="0"/>
+      <c r="XBE34" s="0"/>
+      <c r="XBF34" s="0"/>
+      <c r="XBG34" s="0"/>
+      <c r="XBH34" s="0"/>
+      <c r="XBI34" s="0"/>
+      <c r="XBJ34" s="0"/>
+      <c r="XBK34" s="0"/>
+      <c r="XBL34" s="0"/>
+      <c r="XBM34" s="0"/>
+      <c r="XBN34" s="0"/>
+      <c r="XBO34" s="0"/>
+      <c r="XBP34" s="0"/>
+      <c r="XBQ34" s="0"/>
+      <c r="XBR34" s="0"/>
+      <c r="XBS34" s="0"/>
+      <c r="XBT34" s="0"/>
+      <c r="XBU34" s="0"/>
+      <c r="XBV34" s="0"/>
+      <c r="XBW34" s="0"/>
+      <c r="XBX34" s="0"/>
+      <c r="XBY34" s="0"/>
+      <c r="XBZ34" s="0"/>
+      <c r="XCA34" s="0"/>
+      <c r="XCB34" s="0"/>
+      <c r="XCC34" s="0"/>
+      <c r="XCD34" s="0"/>
+      <c r="XCE34" s="0"/>
+      <c r="XCF34" s="0"/>
+      <c r="XCG34" s="0"/>
+      <c r="XCH34" s="0"/>
+      <c r="XCI34" s="0"/>
+      <c r="XCJ34" s="0"/>
+      <c r="XCK34" s="0"/>
+      <c r="XCL34" s="0"/>
+      <c r="XCM34" s="0"/>
+      <c r="XCN34" s="0"/>
+      <c r="XCO34" s="0"/>
+      <c r="XCP34" s="0"/>
+      <c r="XCQ34" s="0"/>
+      <c r="XCR34" s="0"/>
+      <c r="XCS34" s="0"/>
+      <c r="XCT34" s="0"/>
+      <c r="XCU34" s="0"/>
+      <c r="XCV34" s="0"/>
+      <c r="XCW34" s="0"/>
+      <c r="XCX34" s="0"/>
+      <c r="XCY34" s="0"/>
+      <c r="XCZ34" s="0"/>
+      <c r="XDA34" s="0"/>
+      <c r="XDB34" s="0"/>
+      <c r="XDC34" s="0"/>
+      <c r="XDD34" s="0"/>
+      <c r="XDE34" s="0"/>
+      <c r="XDF34" s="0"/>
+      <c r="XDG34" s="0"/>
+      <c r="XDH34" s="0"/>
+      <c r="XDI34" s="0"/>
+      <c r="XDJ34" s="0"/>
+      <c r="XDK34" s="0"/>
+      <c r="XDL34" s="0"/>
+      <c r="XDM34" s="0"/>
+      <c r="XDN34" s="0"/>
+      <c r="XDO34" s="0"/>
+      <c r="XDP34" s="0"/>
+      <c r="XDQ34" s="0"/>
+      <c r="XDR34" s="0"/>
+      <c r="XDS34" s="0"/>
+      <c r="XDT34" s="0"/>
+      <c r="XDU34" s="0"/>
+      <c r="XDV34" s="0"/>
+      <c r="XDW34" s="0"/>
+      <c r="XDX34" s="0"/>
+      <c r="XDY34" s="0"/>
+      <c r="XDZ34" s="0"/>
+      <c r="XEA34" s="0"/>
+      <c r="XEB34" s="0"/>
+      <c r="XEC34" s="0"/>
+      <c r="XED34" s="0"/>
+      <c r="XEE34" s="0"/>
+      <c r="XEF34" s="0"/>
+      <c r="XEG34" s="0"/>
+      <c r="XEH34" s="0"/>
+      <c r="XEI34" s="0"/>
+      <c r="XEJ34" s="0"/>
+      <c r="XEK34" s="0"/>
+      <c r="XEL34" s="0"/>
+      <c r="XEM34" s="0"/>
+      <c r="XEN34" s="0"/>
+      <c r="XEO34" s="0"/>
+      <c r="XEP34" s="0"/>
+      <c r="XEQ34" s="0"/>
+      <c r="XER34" s="0"/>
+      <c r="XES34" s="0"/>
+      <c r="XET34" s="0"/>
+      <c r="XEU34" s="0"/>
+      <c r="XEV34" s="0"/>
+      <c r="XEW34" s="0"/>
+      <c r="XEX34" s="0"/>
+      <c r="XEY34" s="0"/>
+      <c r="XEZ34" s="0"/>
+      <c r="XFA34" s="0"/>
+      <c r="XFB34" s="0"/>
+      <c r="XFC34" s="0"/>
+      <c r="XFD34" s="0"/>
+    </row>
+    <row r="35" s="61" customFormat="true" ht="75.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="52" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="53" t="n">
+        <v>3504261</v>
+      </c>
+      <c r="E35" s="54" t="n">
+        <v>25829</v>
+      </c>
+      <c r="F35" s="52"/>
+      <c r="G35" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="H35" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="54" t="n">
+        <v>45824</v>
+      </c>
+      <c r="J35" s="54" t="n">
+        <v>45993</v>
+      </c>
+      <c r="K35" s="57" t="n">
+        <v>15</v>
+      </c>
+      <c r="L35" s="58" t="n">
+        <v>2000</v>
+      </c>
+      <c r="M35" s="59" t="n">
+        <f aca="false">ROUND(L35/30*K35,2)</f>
+        <v>1000</v>
+      </c>
+      <c r="N35" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" s="59" t="n">
+        <f aca="false">ROUND(M35-Q35,2)</f>
+        <v>1000</v>
+      </c>
+      <c r="S35" s="52"/>
+      <c r="U35" s="62"/>
+      <c r="V35" s="62"/>
+      <c r="W35" s="62"/>
+      <c r="X35" s="62"/>
+      <c r="Y35" s="62"/>
+      <c r="Z35" s="62"/>
+      <c r="AA35" s="62"/>
+      <c r="AB35" s="62"/>
+      <c r="AC35" s="62"/>
+      <c r="AD35" s="62"/>
+      <c r="AE35" s="62"/>
+      <c r="AF35" s="62"/>
+      <c r="AG35" s="62"/>
+      <c r="AH35" s="62"/>
+      <c r="AI35" s="62"/>
+      <c r="AJ35" s="62"/>
+      <c r="AK35" s="62"/>
+      <c r="AL35" s="62"/>
+      <c r="AM35" s="62"/>
+      <c r="AN35" s="62"/>
+      <c r="AO35" s="62"/>
+      <c r="AP35" s="62"/>
+      <c r="AQ35" s="62"/>
+      <c r="AR35" s="62"/>
+      <c r="AS35" s="62"/>
+      <c r="AT35" s="62"/>
+      <c r="AU35" s="62"/>
+      <c r="AV35" s="62"/>
+      <c r="AW35" s="62"/>
+      <c r="AX35" s="62"/>
+      <c r="AY35" s="62"/>
+      <c r="AZ35" s="62"/>
+      <c r="BA35" s="62"/>
+      <c r="BB35" s="62"/>
+      <c r="BC35" s="62"/>
+      <c r="BD35" s="62"/>
+      <c r="BE35" s="62"/>
+      <c r="BF35" s="62"/>
+      <c r="BG35" s="62"/>
+      <c r="BH35" s="62"/>
+      <c r="BI35" s="62"/>
+      <c r="BJ35" s="62"/>
+      <c r="BK35" s="62"/>
+      <c r="BL35" s="62"/>
+      <c r="BM35" s="62"/>
+      <c r="BN35" s="62"/>
+      <c r="BO35" s="62"/>
+      <c r="BP35" s="62"/>
+      <c r="BQ35" s="62"/>
+      <c r="BR35" s="62"/>
+      <c r="BS35" s="62"/>
+      <c r="BT35" s="62"/>
+      <c r="BU35" s="62"/>
+      <c r="BV35" s="62"/>
+      <c r="BW35" s="62"/>
+      <c r="BX35" s="62"/>
+      <c r="BY35" s="62"/>
+      <c r="BZ35" s="62"/>
+      <c r="CA35" s="62"/>
+      <c r="CB35" s="62"/>
+      <c r="CC35" s="62"/>
+      <c r="CD35" s="62"/>
+      <c r="CE35" s="62"/>
+      <c r="CF35" s="62"/>
+      <c r="CG35" s="62"/>
+      <c r="CH35" s="62"/>
+      <c r="CI35" s="62"/>
+      <c r="CJ35" s="62"/>
+      <c r="CK35" s="62"/>
+      <c r="CL35" s="62"/>
+      <c r="CM35" s="62"/>
+      <c r="CN35" s="62"/>
+      <c r="CO35" s="62"/>
+      <c r="CP35" s="62"/>
+      <c r="CQ35" s="62"/>
+      <c r="CR35" s="62"/>
+      <c r="CS35" s="62"/>
+      <c r="CT35" s="62"/>
+      <c r="CU35" s="62"/>
+      <c r="CV35" s="62"/>
+      <c r="CW35" s="62"/>
+      <c r="CX35" s="62"/>
+      <c r="CY35" s="62"/>
+      <c r="CZ35" s="62"/>
+      <c r="DA35" s="62"/>
+      <c r="DB35" s="62"/>
+      <c r="DC35" s="62"/>
+      <c r="DD35" s="62"/>
+      <c r="DE35" s="62"/>
+      <c r="DF35" s="62"/>
+      <c r="DG35" s="62"/>
+      <c r="DH35" s="62"/>
+      <c r="DI35" s="62"/>
+      <c r="DJ35" s="62"/>
+      <c r="DK35" s="62"/>
+      <c r="DL35" s="62"/>
+      <c r="DM35" s="62"/>
+      <c r="DN35" s="62"/>
+      <c r="DO35" s="62"/>
+      <c r="DP35" s="62"/>
+      <c r="DQ35" s="62"/>
+      <c r="DR35" s="62"/>
+      <c r="DS35" s="62"/>
+      <c r="DT35" s="62"/>
+      <c r="DU35" s="62"/>
+      <c r="DV35" s="62"/>
+      <c r="WUK35" s="0"/>
+      <c r="WUL35" s="0"/>
+      <c r="WUM35" s="0"/>
+      <c r="WUN35" s="0"/>
+      <c r="WUO35" s="0"/>
+      <c r="WUP35" s="0"/>
+      <c r="WUQ35" s="0"/>
+      <c r="WUR35" s="0"/>
+      <c r="WUS35" s="0"/>
+      <c r="WUT35" s="0"/>
+      <c r="WUU35" s="0"/>
+      <c r="WUV35" s="0"/>
+      <c r="WUW35" s="0"/>
+      <c r="WUX35" s="0"/>
+      <c r="WUY35" s="0"/>
+      <c r="WUZ35" s="0"/>
+      <c r="WVA35" s="0"/>
+      <c r="WVB35" s="0"/>
+      <c r="WVC35" s="0"/>
+      <c r="WVD35" s="0"/>
+      <c r="WVE35" s="0"/>
+      <c r="WVF35" s="0"/>
+      <c r="WVG35" s="0"/>
+      <c r="WVH35" s="0"/>
+      <c r="WVI35" s="0"/>
+      <c r="WVJ35" s="0"/>
+      <c r="WVK35" s="0"/>
+      <c r="WVL35" s="0"/>
+      <c r="WVM35" s="0"/>
+      <c r="WVN35" s="0"/>
+      <c r="WVO35" s="0"/>
+      <c r="WVP35" s="0"/>
+      <c r="WVQ35" s="0"/>
+      <c r="WVR35" s="0"/>
+      <c r="WVS35" s="0"/>
+      <c r="WVT35" s="0"/>
+      <c r="WVU35" s="0"/>
+      <c r="WVV35" s="0"/>
+      <c r="WVW35" s="0"/>
+      <c r="WVX35" s="0"/>
+      <c r="WVY35" s="0"/>
+      <c r="WVZ35" s="0"/>
+      <c r="WWA35" s="0"/>
+      <c r="WWB35" s="0"/>
+      <c r="WWC35" s="0"/>
+      <c r="WWD35" s="0"/>
+      <c r="WWE35" s="0"/>
+      <c r="WWF35" s="0"/>
+      <c r="WWG35" s="0"/>
+      <c r="WWH35" s="0"/>
+      <c r="WWI35" s="0"/>
+      <c r="WWJ35" s="0"/>
+      <c r="WWK35" s="0"/>
+      <c r="WWL35" s="0"/>
+      <c r="WWM35" s="0"/>
+      <c r="WWN35" s="0"/>
+      <c r="WWO35" s="0"/>
+      <c r="WWP35" s="0"/>
+      <c r="WWQ35" s="0"/>
+      <c r="WWR35" s="0"/>
+      <c r="WWS35" s="0"/>
+      <c r="WWT35" s="0"/>
+      <c r="WWU35" s="0"/>
+      <c r="WWV35" s="0"/>
+      <c r="WWW35" s="0"/>
+      <c r="WWX35" s="0"/>
+      <c r="WWY35" s="0"/>
+      <c r="WWZ35" s="0"/>
+      <c r="WXA35" s="0"/>
+      <c r="WXB35" s="0"/>
+      <c r="WXC35" s="0"/>
+      <c r="WXD35" s="0"/>
+      <c r="WXE35" s="0"/>
+      <c r="WXF35" s="0"/>
+      <c r="WXG35" s="0"/>
+      <c r="WXH35" s="0"/>
+      <c r="WXI35" s="0"/>
+      <c r="WXJ35" s="0"/>
+      <c r="WXK35" s="0"/>
+      <c r="WXL35" s="0"/>
+      <c r="WXM35" s="0"/>
+      <c r="WXN35" s="0"/>
+      <c r="WXO35" s="0"/>
+      <c r="WXP35" s="0"/>
+      <c r="WXQ35" s="0"/>
+      <c r="WXR35" s="0"/>
+      <c r="WXS35" s="0"/>
+      <c r="WXT35" s="0"/>
+      <c r="WXU35" s="0"/>
+      <c r="WXV35" s="0"/>
+      <c r="WXW35" s="0"/>
+      <c r="WXX35" s="0"/>
+      <c r="WXY35" s="0"/>
+      <c r="WXZ35" s="0"/>
+      <c r="WYA35" s="0"/>
+      <c r="WYB35" s="0"/>
+      <c r="WYC35" s="0"/>
+      <c r="WYD35" s="0"/>
+      <c r="WYE35" s="0"/>
+      <c r="WYF35" s="0"/>
+      <c r="WYG35" s="0"/>
+      <c r="WYH35" s="0"/>
+      <c r="WYI35" s="0"/>
+      <c r="WYJ35" s="0"/>
+      <c r="WYK35" s="0"/>
+      <c r="WYL35" s="0"/>
+      <c r="WYM35" s="0"/>
+      <c r="WYN35" s="0"/>
+      <c r="WYO35" s="0"/>
+      <c r="WYP35" s="0"/>
+      <c r="WYQ35" s="0"/>
+      <c r="WYR35" s="0"/>
+      <c r="WYS35" s="0"/>
+      <c r="WYT35" s="0"/>
+      <c r="WYU35" s="0"/>
+      <c r="WYV35" s="0"/>
+      <c r="WYW35" s="0"/>
+      <c r="WYX35" s="0"/>
+      <c r="WYY35" s="0"/>
+      <c r="WYZ35" s="0"/>
+      <c r="WZA35" s="0"/>
+      <c r="WZB35" s="0"/>
+      <c r="WZC35" s="0"/>
+      <c r="WZD35" s="0"/>
+      <c r="WZE35" s="0"/>
+      <c r="WZF35" s="0"/>
+      <c r="WZG35" s="0"/>
+      <c r="WZH35" s="0"/>
+      <c r="WZI35" s="0"/>
+      <c r="WZJ35" s="0"/>
+      <c r="WZK35" s="0"/>
+      <c r="WZL35" s="0"/>
+      <c r="WZM35" s="0"/>
+      <c r="WZN35" s="0"/>
+      <c r="WZO35" s="0"/>
+      <c r="WZP35" s="0"/>
+      <c r="WZQ35" s="0"/>
+      <c r="WZR35" s="0"/>
+      <c r="WZS35" s="0"/>
+      <c r="WZT35" s="0"/>
+      <c r="WZU35" s="0"/>
+      <c r="WZV35" s="0"/>
+      <c r="WZW35" s="0"/>
+      <c r="WZX35" s="0"/>
+      <c r="WZY35" s="0"/>
+      <c r="WZZ35" s="0"/>
+      <c r="XAA35" s="0"/>
+      <c r="XAB35" s="0"/>
+      <c r="XAC35" s="0"/>
+      <c r="XAD35" s="0"/>
+      <c r="XAE35" s="0"/>
+      <c r="XAF35" s="0"/>
+      <c r="XAG35" s="0"/>
+      <c r="XAH35" s="0"/>
+      <c r="XAI35" s="0"/>
+      <c r="XAJ35" s="0"/>
+      <c r="XAK35" s="0"/>
+      <c r="XAL35" s="0"/>
+      <c r="XAM35" s="0"/>
+      <c r="XAN35" s="0"/>
+      <c r="XAO35" s="0"/>
+      <c r="XAP35" s="0"/>
+      <c r="XAQ35" s="0"/>
+      <c r="XAR35" s="0"/>
+      <c r="XAS35" s="0"/>
+      <c r="XAT35" s="0"/>
+      <c r="XAU35" s="0"/>
+      <c r="XAV35" s="0"/>
+      <c r="XAW35" s="0"/>
+      <c r="XAX35" s="0"/>
+      <c r="XAY35" s="0"/>
+      <c r="XAZ35" s="0"/>
+      <c r="XBA35" s="0"/>
+      <c r="XBB35" s="0"/>
+      <c r="XBC35" s="0"/>
+      <c r="XBD35" s="0"/>
+      <c r="XBE35" s="0"/>
+      <c r="XBF35" s="0"/>
+      <c r="XBG35" s="0"/>
+      <c r="XBH35" s="0"/>
+      <c r="XBI35" s="0"/>
+      <c r="XBJ35" s="0"/>
+      <c r="XBK35" s="0"/>
+      <c r="XBL35" s="0"/>
+      <c r="XBM35" s="0"/>
+      <c r="XBN35" s="0"/>
+      <c r="XBO35" s="0"/>
+      <c r="XBP35" s="0"/>
+      <c r="XBQ35" s="0"/>
+      <c r="XBR35" s="0"/>
+      <c r="XBS35" s="0"/>
+      <c r="XBT35" s="0"/>
+      <c r="XBU35" s="0"/>
+      <c r="XBV35" s="0"/>
+      <c r="XBW35" s="0"/>
+      <c r="XBX35" s="0"/>
+      <c r="XBY35" s="0"/>
+      <c r="XBZ35" s="0"/>
+      <c r="XCA35" s="0"/>
+      <c r="XCB35" s="0"/>
+      <c r="XCC35" s="0"/>
+      <c r="XCD35" s="0"/>
+      <c r="XCE35" s="0"/>
+      <c r="XCF35" s="0"/>
+      <c r="XCG35" s="0"/>
+      <c r="XCH35" s="0"/>
+      <c r="XCI35" s="0"/>
+      <c r="XCJ35" s="0"/>
+      <c r="XCK35" s="0"/>
+      <c r="XCL35" s="0"/>
+      <c r="XCM35" s="0"/>
+      <c r="XCN35" s="0"/>
+      <c r="XCO35" s="0"/>
+      <c r="XCP35" s="0"/>
+      <c r="XCQ35" s="0"/>
+      <c r="XCR35" s="0"/>
+      <c r="XCS35" s="0"/>
+      <c r="XCT35" s="0"/>
+      <c r="XCU35" s="0"/>
+      <c r="XCV35" s="0"/>
+      <c r="XCW35" s="0"/>
+      <c r="XCX35" s="0"/>
+      <c r="XCY35" s="0"/>
+      <c r="XCZ35" s="0"/>
+      <c r="XDA35" s="0"/>
+      <c r="XDB35" s="0"/>
+      <c r="XDC35" s="0"/>
+      <c r="XDD35" s="0"/>
+      <c r="XDE35" s="0"/>
+      <c r="XDF35" s="0"/>
+      <c r="XDG35" s="0"/>
+      <c r="XDH35" s="0"/>
+      <c r="XDI35" s="0"/>
+      <c r="XDJ35" s="0"/>
+      <c r="XDK35" s="0"/>
+      <c r="XDL35" s="0"/>
+      <c r="XDM35" s="0"/>
+      <c r="XDN35" s="0"/>
+      <c r="XDO35" s="0"/>
+      <c r="XDP35" s="0"/>
+      <c r="XDQ35" s="0"/>
+      <c r="XDR35" s="0"/>
+      <c r="XDS35" s="0"/>
+      <c r="XDT35" s="0"/>
+      <c r="XDU35" s="0"/>
+      <c r="XDV35" s="0"/>
+      <c r="XDW35" s="0"/>
+      <c r="XDX35" s="0"/>
+      <c r="XDY35" s="0"/>
+      <c r="XDZ35" s="0"/>
+      <c r="XEA35" s="0"/>
+      <c r="XEB35" s="0"/>
+      <c r="XEC35" s="0"/>
+      <c r="XED35" s="0"/>
+      <c r="XEE35" s="0"/>
+      <c r="XEF35" s="0"/>
+      <c r="XEG35" s="0"/>
+      <c r="XEH35" s="0"/>
+      <c r="XEI35" s="0"/>
+      <c r="XEJ35" s="0"/>
+      <c r="XEK35" s="0"/>
+      <c r="XEL35" s="0"/>
+      <c r="XEM35" s="0"/>
+      <c r="XEN35" s="0"/>
+      <c r="XEO35" s="0"/>
+      <c r="XEP35" s="0"/>
+      <c r="XEQ35" s="0"/>
+      <c r="XER35" s="0"/>
+      <c r="XES35" s="0"/>
+      <c r="XET35" s="0"/>
+      <c r="XEU35" s="0"/>
+      <c r="XEV35" s="0"/>
+      <c r="XEW35" s="0"/>
+      <c r="XEX35" s="0"/>
+      <c r="XEY35" s="0"/>
+      <c r="XEZ35" s="0"/>
+      <c r="XFA35" s="0"/>
+      <c r="XFB35" s="0"/>
+      <c r="XFC35" s="0"/>
+      <c r="XFD35" s="0"/>
+    </row>
+    <row r="36" s="65" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="64" t="n">
+        <f aca="false">SUM(L34:L35)</f>
+        <v>4000</v>
+      </c>
+      <c r="M36" s="64" t="n">
+        <f aca="false">SUM(M34:M35)</f>
+        <v>2000</v>
+      </c>
+      <c r="N36" s="64" t="n">
+        <f aca="false">SUM(N34:N35)</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="64" t="n">
+        <f aca="false">SUM(O34:O35)</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="64" t="n">
+        <f aca="false">SUM(P34:P35)</f>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="64" t="n">
+        <f aca="false">SUM(Q34:Q35)</f>
+        <v>0</v>
+      </c>
+      <c r="R36" s="64" t="n">
+        <f aca="false">SUM(R34:R35)</f>
+        <v>2000</v>
+      </c>
+      <c r="S36" s="64"/>
+      <c r="U36" s="66"/>
+      <c r="V36" s="66"/>
+      <c r="W36" s="66"/>
+      <c r="X36" s="66"/>
+      <c r="Y36" s="66"/>
+      <c r="Z36" s="66"/>
+      <c r="AA36" s="66"/>
+      <c r="AB36" s="66"/>
+      <c r="AC36" s="66"/>
+      <c r="AD36" s="66"/>
+      <c r="AE36" s="66"/>
+      <c r="AF36" s="66"/>
+      <c r="AG36" s="66"/>
+      <c r="AH36" s="66"/>
+      <c r="AI36" s="66"/>
+      <c r="AJ36" s="66"/>
+      <c r="AK36" s="66"/>
+      <c r="AL36" s="66"/>
+      <c r="AM36" s="66"/>
+      <c r="AN36" s="66"/>
+      <c r="AO36" s="66"/>
+      <c r="AP36" s="66"/>
+      <c r="AQ36" s="66"/>
+      <c r="AR36" s="66"/>
+      <c r="AS36" s="66"/>
+      <c r="AT36" s="66"/>
+      <c r="AU36" s="66"/>
+      <c r="AV36" s="66"/>
+      <c r="AW36" s="66"/>
+      <c r="AX36" s="66"/>
+      <c r="AY36" s="66"/>
+      <c r="AZ36" s="66"/>
+      <c r="BA36" s="66"/>
+      <c r="BB36" s="66"/>
+      <c r="BC36" s="66"/>
+      <c r="BD36" s="66"/>
+      <c r="BE36" s="66"/>
+      <c r="BF36" s="66"/>
+      <c r="BG36" s="66"/>
+      <c r="BH36" s="66"/>
+      <c r="BI36" s="66"/>
+      <c r="BJ36" s="66"/>
+      <c r="BK36" s="66"/>
+      <c r="BL36" s="66"/>
+      <c r="BM36" s="66"/>
+      <c r="BN36" s="66"/>
+      <c r="BO36" s="66"/>
+      <c r="BP36" s="66"/>
+      <c r="BQ36" s="66"/>
+      <c r="BR36" s="66"/>
+      <c r="BS36" s="66"/>
+      <c r="BT36" s="66"/>
+      <c r="BU36" s="66"/>
+      <c r="BV36" s="66"/>
+      <c r="BW36" s="66"/>
+      <c r="BX36" s="66"/>
+      <c r="BY36" s="66"/>
+      <c r="BZ36" s="66"/>
+      <c r="CA36" s="66"/>
+      <c r="CB36" s="66"/>
+      <c r="CC36" s="66"/>
+      <c r="CD36" s="66"/>
+      <c r="CE36" s="66"/>
+      <c r="CF36" s="66"/>
+      <c r="CG36" s="66"/>
+      <c r="CH36" s="66"/>
+      <c r="CI36" s="66"/>
+      <c r="CJ36" s="66"/>
+      <c r="CK36" s="66"/>
+      <c r="CL36" s="66"/>
+      <c r="CM36" s="66"/>
+      <c r="CN36" s="66"/>
+      <c r="CO36" s="66"/>
+      <c r="CP36" s="66"/>
+      <c r="CQ36" s="66"/>
+      <c r="CR36" s="66"/>
+      <c r="CS36" s="66"/>
+      <c r="CT36" s="66"/>
+      <c r="CU36" s="66"/>
+      <c r="CV36" s="66"/>
+      <c r="CW36" s="66"/>
+      <c r="CX36" s="66"/>
+      <c r="CY36" s="66"/>
+      <c r="CZ36" s="66"/>
+      <c r="DA36" s="66"/>
+      <c r="DB36" s="66"/>
+      <c r="DC36" s="66"/>
+      <c r="DD36" s="66"/>
+      <c r="DE36" s="66"/>
+      <c r="DF36" s="66"/>
+      <c r="DG36" s="66"/>
+      <c r="DH36" s="66"/>
+      <c r="DI36" s="66"/>
+      <c r="DJ36" s="66"/>
+      <c r="DK36" s="66"/>
+      <c r="DL36" s="66"/>
+      <c r="DM36" s="66"/>
+      <c r="DN36" s="66"/>
+      <c r="DO36" s="66"/>
+      <c r="DP36" s="66"/>
+      <c r="DQ36" s="66"/>
+      <c r="DR36" s="66"/>
+      <c r="DS36" s="66"/>
+      <c r="DT36" s="66"/>
+      <c r="DU36" s="66"/>
+      <c r="DV36" s="66"/>
+      <c r="WUK36" s="0"/>
+      <c r="WUL36" s="0"/>
+      <c r="WUM36" s="0"/>
+      <c r="WUN36" s="0"/>
+      <c r="WUO36" s="0"/>
+      <c r="WUP36" s="0"/>
+      <c r="WUQ36" s="0"/>
+      <c r="WUR36" s="0"/>
+      <c r="WUS36" s="0"/>
+      <c r="WUT36" s="0"/>
+      <c r="WUU36" s="0"/>
+      <c r="WUV36" s="0"/>
+      <c r="WUW36" s="0"/>
+      <c r="WUX36" s="0"/>
+      <c r="WUY36" s="0"/>
+      <c r="WUZ36" s="0"/>
+      <c r="WVA36" s="0"/>
+      <c r="WVB36" s="0"/>
+      <c r="WVC36" s="0"/>
+      <c r="WVD36" s="0"/>
+      <c r="WVE36" s="0"/>
+      <c r="WVF36" s="0"/>
+      <c r="WVG36" s="0"/>
+      <c r="WVH36" s="0"/>
+      <c r="WVI36" s="0"/>
+      <c r="WVJ36" s="0"/>
+      <c r="WVK36" s="0"/>
+      <c r="WVL36" s="0"/>
+      <c r="WVM36" s="0"/>
+      <c r="WVN36" s="0"/>
+      <c r="WVO36" s="0"/>
+      <c r="WVP36" s="0"/>
+      <c r="WVQ36" s="0"/>
+      <c r="WVR36" s="0"/>
+      <c r="WVS36" s="0"/>
+      <c r="WVT36" s="0"/>
+      <c r="WVU36" s="0"/>
+      <c r="WVV36" s="0"/>
+      <c r="WVW36" s="0"/>
+      <c r="WVX36" s="0"/>
+      <c r="WVY36" s="0"/>
+      <c r="WVZ36" s="0"/>
+      <c r="WWA36" s="0"/>
+      <c r="WWB36" s="0"/>
+      <c r="WWC36" s="0"/>
+      <c r="WWD36" s="0"/>
+      <c r="WWE36" s="0"/>
+      <c r="WWF36" s="0"/>
+      <c r="WWG36" s="0"/>
+      <c r="WWH36" s="0"/>
+      <c r="WWI36" s="0"/>
+      <c r="WWJ36" s="0"/>
+      <c r="WWK36" s="0"/>
+      <c r="WWL36" s="0"/>
+      <c r="WWM36" s="0"/>
+      <c r="WWN36" s="0"/>
+      <c r="WWO36" s="0"/>
+      <c r="WWP36" s="0"/>
+      <c r="WWQ36" s="0"/>
+      <c r="WWR36" s="0"/>
+      <c r="WWS36" s="0"/>
+      <c r="WWT36" s="0"/>
+      <c r="WWU36" s="0"/>
+      <c r="WWV36" s="0"/>
+      <c r="WWW36" s="0"/>
+      <c r="WWX36" s="0"/>
+      <c r="WWY36" s="0"/>
+      <c r="WWZ36" s="0"/>
+      <c r="WXA36" s="0"/>
+      <c r="WXB36" s="0"/>
+      <c r="WXC36" s="0"/>
+      <c r="WXD36" s="0"/>
+      <c r="WXE36" s="0"/>
+      <c r="WXF36" s="0"/>
+      <c r="WXG36" s="0"/>
+      <c r="WXH36" s="0"/>
+      <c r="WXI36" s="0"/>
+      <c r="WXJ36" s="0"/>
+      <c r="WXK36" s="0"/>
+      <c r="WXL36" s="0"/>
+      <c r="WXM36" s="0"/>
+      <c r="WXN36" s="0"/>
+      <c r="WXO36" s="0"/>
+      <c r="WXP36" s="0"/>
+      <c r="WXQ36" s="0"/>
+      <c r="WXR36" s="0"/>
+      <c r="WXS36" s="0"/>
+      <c r="WXT36" s="0"/>
+      <c r="WXU36" s="0"/>
+      <c r="WXV36" s="0"/>
+      <c r="WXW36" s="0"/>
+      <c r="WXX36" s="0"/>
+      <c r="WXY36" s="0"/>
+      <c r="WXZ36" s="0"/>
+      <c r="WYA36" s="0"/>
+      <c r="WYB36" s="0"/>
+      <c r="WYC36" s="0"/>
+      <c r="WYD36" s="0"/>
+      <c r="WYE36" s="0"/>
+      <c r="WYF36" s="0"/>
+      <c r="WYG36" s="0"/>
+      <c r="WYH36" s="0"/>
+      <c r="WYI36" s="0"/>
+      <c r="WYJ36" s="0"/>
+      <c r="WYK36" s="0"/>
+      <c r="WYL36" s="0"/>
+      <c r="WYM36" s="0"/>
+      <c r="WYN36" s="0"/>
+      <c r="WYO36" s="0"/>
+      <c r="WYP36" s="0"/>
+      <c r="WYQ36" s="0"/>
+      <c r="WYR36" s="0"/>
+      <c r="WYS36" s="0"/>
+      <c r="WYT36" s="0"/>
+      <c r="WYU36" s="0"/>
+      <c r="WYV36" s="0"/>
+      <c r="WYW36" s="0"/>
+      <c r="WYX36" s="0"/>
+      <c r="WYY36" s="0"/>
+      <c r="WYZ36" s="0"/>
+      <c r="WZA36" s="0"/>
+      <c r="WZB36" s="0"/>
+      <c r="WZC36" s="0"/>
+      <c r="WZD36" s="0"/>
+      <c r="WZE36" s="0"/>
+      <c r="WZF36" s="0"/>
+      <c r="WZG36" s="0"/>
+      <c r="WZH36" s="0"/>
+      <c r="WZI36" s="0"/>
+      <c r="WZJ36" s="0"/>
+      <c r="WZK36" s="0"/>
+      <c r="WZL36" s="0"/>
+      <c r="WZM36" s="0"/>
+      <c r="WZN36" s="0"/>
+      <c r="WZO36" s="0"/>
+      <c r="WZP36" s="0"/>
+      <c r="WZQ36" s="0"/>
+      <c r="WZR36" s="0"/>
+      <c r="WZS36" s="0"/>
+      <c r="WZT36" s="0"/>
+      <c r="WZU36" s="0"/>
+      <c r="WZV36" s="0"/>
+      <c r="WZW36" s="0"/>
+      <c r="WZX36" s="0"/>
+      <c r="WZY36" s="0"/>
+      <c r="WZZ36" s="0"/>
+      <c r="XAA36" s="0"/>
+      <c r="XAB36" s="0"/>
+      <c r="XAC36" s="0"/>
+      <c r="XAD36" s="0"/>
+      <c r="XAE36" s="0"/>
+      <c r="XAF36" s="0"/>
+      <c r="XAG36" s="0"/>
+      <c r="XAH36" s="0"/>
+      <c r="XAI36" s="0"/>
+      <c r="XAJ36" s="0"/>
+      <c r="XAK36" s="0"/>
+      <c r="XAL36" s="0"/>
+      <c r="XAM36" s="0"/>
+      <c r="XAN36" s="0"/>
+      <c r="XAO36" s="0"/>
+      <c r="XAP36" s="0"/>
+      <c r="XAQ36" s="0"/>
+      <c r="XAR36" s="0"/>
+      <c r="XAS36" s="0"/>
+      <c r="XAT36" s="0"/>
+      <c r="XAU36" s="0"/>
+      <c r="XAV36" s="0"/>
+      <c r="XAW36" s="0"/>
+      <c r="XAX36" s="0"/>
+      <c r="XAY36" s="0"/>
+      <c r="XAZ36" s="0"/>
+      <c r="XBA36" s="0"/>
+      <c r="XBB36" s="0"/>
+      <c r="XBC36" s="0"/>
+      <c r="XBD36" s="0"/>
+      <c r="XBE36" s="0"/>
+      <c r="XBF36" s="0"/>
+      <c r="XBG36" s="0"/>
+      <c r="XBH36" s="0"/>
+      <c r="XBI36" s="0"/>
+      <c r="XBJ36" s="0"/>
+      <c r="XBK36" s="0"/>
+      <c r="XBL36" s="0"/>
+      <c r="XBM36" s="0"/>
+      <c r="XBN36" s="0"/>
+      <c r="XBO36" s="0"/>
+      <c r="XBP36" s="0"/>
+      <c r="XBQ36" s="0"/>
+      <c r="XBR36" s="0"/>
+      <c r="XBS36" s="0"/>
+      <c r="XBT36" s="0"/>
+      <c r="XBU36" s="0"/>
+      <c r="XBV36" s="0"/>
+      <c r="XBW36" s="0"/>
+      <c r="XBX36" s="0"/>
+      <c r="XBY36" s="0"/>
+      <c r="XBZ36" s="0"/>
+      <c r="XCA36" s="0"/>
+      <c r="XCB36" s="0"/>
+      <c r="XCC36" s="0"/>
+      <c r="XCD36" s="0"/>
+      <c r="XCE36" s="0"/>
+      <c r="XCF36" s="0"/>
+      <c r="XCG36" s="0"/>
+      <c r="XCH36" s="0"/>
+      <c r="XCI36" s="0"/>
+      <c r="XCJ36" s="0"/>
+      <c r="XCK36" s="0"/>
+      <c r="XCL36" s="0"/>
+      <c r="XCM36" s="0"/>
+      <c r="XCN36" s="0"/>
+      <c r="XCO36" s="0"/>
+      <c r="XCP36" s="0"/>
+      <c r="XCQ36" s="0"/>
+      <c r="XCR36" s="0"/>
+      <c r="XCS36" s="0"/>
+      <c r="XCT36" s="0"/>
+      <c r="XCU36" s="0"/>
+      <c r="XCV36" s="0"/>
+      <c r="XCW36" s="0"/>
+      <c r="XCX36" s="0"/>
+      <c r="XCY36" s="0"/>
+      <c r="XCZ36" s="0"/>
+      <c r="XDA36" s="0"/>
+      <c r="XDB36" s="0"/>
+      <c r="XDC36" s="0"/>
+      <c r="XDD36" s="0"/>
+      <c r="XDE36" s="0"/>
+      <c r="XDF36" s="0"/>
+      <c r="XDG36" s="0"/>
+      <c r="XDH36" s="0"/>
+      <c r="XDI36" s="0"/>
+      <c r="XDJ36" s="0"/>
+      <c r="XDK36" s="0"/>
+      <c r="XDL36" s="0"/>
+      <c r="XDM36" s="0"/>
+      <c r="XDN36" s="0"/>
+      <c r="XDO36" s="0"/>
+      <c r="XDP36" s="0"/>
+      <c r="XDQ36" s="0"/>
+      <c r="XDR36" s="0"/>
+      <c r="XDS36" s="0"/>
+      <c r="XDT36" s="0"/>
+      <c r="XDU36" s="0"/>
+      <c r="XDV36" s="0"/>
+      <c r="XDW36" s="0"/>
+      <c r="XDX36" s="0"/>
+      <c r="XDY36" s="0"/>
+      <c r="XDZ36" s="0"/>
+      <c r="XEA36" s="0"/>
+      <c r="XEB36" s="0"/>
+      <c r="XEC36" s="0"/>
+      <c r="XED36" s="0"/>
+      <c r="XEE36" s="0"/>
+      <c r="XEF36" s="0"/>
+      <c r="XEG36" s="0"/>
+      <c r="XEH36" s="0"/>
+      <c r="XEI36" s="0"/>
+      <c r="XEJ36" s="0"/>
+      <c r="XEK36" s="0"/>
+      <c r="XEL36" s="0"/>
+      <c r="XEM36" s="0"/>
+      <c r="XEN36" s="0"/>
+      <c r="XEO36" s="0"/>
+      <c r="XEP36" s="0"/>
+      <c r="XEQ36" s="0"/>
+      <c r="XER36" s="0"/>
+      <c r="XES36" s="0"/>
+      <c r="XET36" s="0"/>
+      <c r="XEU36" s="0"/>
+      <c r="XEV36" s="0"/>
+      <c r="XEW36" s="0"/>
+      <c r="XEX36" s="0"/>
+      <c r="XEY36" s="0"/>
+      <c r="XEZ36" s="0"/>
+      <c r="XFA36" s="0"/>
+      <c r="XFB36" s="0"/>
+      <c r="XFC36" s="0"/>
+      <c r="XFD36" s="0"/>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
     <mergeCell ref="A5:S5"/>
     <mergeCell ref="A6:S6"/>
     <mergeCell ref="A7:S7"/>
@@ -34013,6 +35697,8 @@
     <mergeCell ref="A11:S11"/>
     <mergeCell ref="A28:S28"/>
     <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A33:S33"/>
+    <mergeCell ref="A36:K36"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.39375" top="0.590277777777778" bottom="0.340277777777778" header="0.511811023622047" footer="0.315277777777778"/>
@@ -34035,7 +35721,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="1" sqref="33:36 A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34047,8 +35733,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="3" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="14.29"/>

</xml_diff>